<commit_message>
Update Cases and Check-list
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="291">
   <si>
     <t>ID</t>
   </si>
@@ -67,7 +67,7 @@
     <t>ТК2</t>
   </si>
   <si>
-    <t>Авторизация в приложении (негативный сценарий)</t>
+    <t>Авторизация в приложении. Негативный сценарий, неверный логин.</t>
   </si>
   <si>
     <t>1. Ввести в поле "Login" данные: login.</t>
@@ -82,7 +82,7 @@
     <t>ТК3</t>
   </si>
   <si>
-    <t>1. Ввести в поле "Login2" данные: login.</t>
+    <t>Авторизация в приложении. Негативный сценарий, неверный пароль.</t>
   </si>
   <si>
     <t>2. Ввести в поле "Password" данные: password.</t>
@@ -373,7 +373,7 @@
     <t>7. Нажать на кнопку "Save".</t>
   </si>
   <si>
-    <t>7. Открылся экран "Control panel", добавлена новость в введеными данными.</t>
+    <t>7. Открылся экран "Control panel", добавлена новость с введеными данными.</t>
   </si>
   <si>
     <t>ТК18</t>
@@ -649,7 +649,7 @@
     <t>1. Ввести в поле "Login" данные: "логин".</t>
   </si>
   <si>
-    <t>1. Данные не ввелись.</t>
+    <t>1. Нет ошибок валидации</t>
   </si>
   <si>
     <t>2. Ввести в поле "Password" данные: "пароль".</t>
@@ -664,10 +664,40 @@
     <t>Ввод данных на кириллице при создании новости.</t>
   </si>
   <si>
-    <t>1. Ввести в поле "Title" данные: "заголовок".</t>
-  </si>
-  <si>
-    <t>2. Ввести в поле "Desctiption" данные: "описание".</t>
+    <t>1. Нажать на поле "Category"</t>
+  </si>
+  <si>
+    <t>1. Открылся выпадающий список с категориями.</t>
+  </si>
+  <si>
+    <t>2. Из выпадающего списка поля "category" выбрать категорию "Объявление".</t>
+  </si>
+  <si>
+    <t>2. В поле "category" появилось значение "Объявление", в поле "Title" появилось значение "Объявление".</t>
+  </si>
+  <si>
+    <t>3. В поле "Publication date" выбрать текущую дату.</t>
+  </si>
+  <si>
+    <t>3. В поле "Publication date" появилась текущая дата.</t>
+  </si>
+  <si>
+    <t>4. В поле "Time" выбрать текущее время.</t>
+  </si>
+  <si>
+    <t>4. В поле "Time" появилось текущее время.</t>
+  </si>
+  <si>
+    <t>5. В поле "Description" ввксти строку "описание".</t>
+  </si>
+  <si>
+    <t>5. В поле "Description появилось значение "decscription".</t>
+  </si>
+  <si>
+    <t>6. Нажать на кнопку "Save".</t>
+  </si>
+  <si>
+    <t>6. Открылся экран "Control panel", добавлена новость с введеными данными.</t>
   </si>
   <si>
     <t>ТК28</t>
@@ -676,10 +706,181 @@
     <t>Ввод данных на кириллице при редактироввании новости.</t>
   </si>
   <si>
+    <t>ТК29</t>
+  </si>
+  <si>
+    <t>Авторизация в приложении. Негативный сценарий, пустое значение в поле логин.</t>
+  </si>
+  <si>
+    <t>1. Ввести в поле "Password" данные: password.</t>
+  </si>
+  <si>
+    <t>2. Нажать кнопку "Sign in".</t>
+  </si>
+  <si>
+    <t>2. Отобразилось всплывающее окно с текстом: "Логин и пароль не могут быть пустыми".</t>
+  </si>
+  <si>
+    <t>ТК30</t>
+  </si>
+  <si>
+    <t>ТК31</t>
+  </si>
+  <si>
+    <t>Фильтрация новостей на экране "News". Негативный сценарий, период фильтрации.</t>
+  </si>
+  <si>
+    <t>2. В первом поле даты выбрать текущую дату.</t>
+  </si>
+  <si>
+    <t>2. В первом поле даты появилась текущая дата.</t>
+  </si>
+  <si>
+    <t>3. Во втором поле даты выбрать дату на три дня ранее даты в первом поле.</t>
+  </si>
+  <si>
+    <t>3. На виджете календарь невозможно выбрать дату ранее даты в первом поле.</t>
+  </si>
+  <si>
+    <t>ТК32</t>
+  </si>
+  <si>
+    <t>Фильтрация новостей на экране "Control panel". Негативный сценарий, период фильтрации.</t>
+  </si>
+  <si>
+    <t>ТК33</t>
+  </si>
+  <si>
+    <t>Добавление новости. Негативный сценарий, дата и время публикации.</t>
+  </si>
+  <si>
+    <t>4. В поле "Publication date" выбрать дату на три дня ранее текущей.</t>
+  </si>
+  <si>
+    <t>4. На виджете календарь невозможно выбрать дату ранее даты ранее текущей.</t>
+  </si>
+  <si>
+    <t>5. В поле "Time" выбрать время на три часа ранее текущего</t>
+  </si>
+  <si>
+    <t>5. На виджете время невозможно выбрать время ранее текущего.</t>
+  </si>
+  <si>
+    <t>ТК34</t>
+  </si>
+  <si>
+    <t>Редактирование существующей новости. Негативный сценарий, дата и время публикации.</t>
+  </si>
+  <si>
+    <t>5. В поле "Publication date" выбрать дату на три дня ранее текущей.</t>
+  </si>
+  <si>
+    <t>5. На виджете календарь невозможно выбрать дату ранее даты ранее текущей.</t>
+  </si>
+  <si>
+    <t>6. В поле "Time" выбрать время на три часа ранее текущего</t>
+  </si>
+  <si>
+    <t>6. На виджете время невозможно выбрать время ранее текущего.</t>
+  </si>
+  <si>
+    <t>ТК35</t>
+  </si>
+  <si>
+    <t>Фильтрация новостей на экране "Control panel". Негативный сценарий, активные и неактивные новости.</t>
+  </si>
+  <si>
+    <t>7. Нажать на чек бокс "Not active"</t>
+  </si>
+  <si>
+    <t>7. Чек бокс "Not active" очищен.</t>
+  </si>
+  <si>
+    <t>8. Нажать кнопку "Filter".</t>
+  </si>
+  <si>
+    <t>8. На экране "Control panel" показаны новости соответствующие фильтрации.</t>
+  </si>
+  <si>
+    <t>ТК36</t>
+  </si>
+  <si>
+    <t>Переход с экрана Main на экран News. Негативный сценарий, потеря интернет соединения.</t>
+  </si>
+  <si>
+    <t>Открыто приложение "Вхосписе", произведена авторизация, открыт экран "Main", отключено интернет соединение.</t>
+  </si>
+  <si>
+    <t>2. Открылся экран "News". Появилось всплывающее сообщение: "Something went wrong. Try again later".</t>
+  </si>
+  <si>
+    <t>ТК37</t>
+  </si>
+  <si>
+    <t>Переход с экрана Main на экран About. Негативный сценарий, потеря интернет соединения.</t>
+  </si>
+  <si>
+    <t>2. Открылся экран "About". Появилось всплывающее сообщение: "Something went wrong. Try again later".</t>
+  </si>
+  <si>
+    <t>ТК38</t>
+  </si>
+  <si>
+    <t>Переход с экрана News на экран Main. Негативный сценарий, потеря интернет соединения.</t>
+  </si>
+  <si>
+    <t>Открыто приложение "Вхосписе", произведена авторизация и открыт экран "News", отключено интернет соединение.</t>
+  </si>
+  <si>
+    <t>2. Открылся экран "Main". Появилось всплывающее сообщение: "Something went wrong. Try again later".</t>
+  </si>
+  <si>
+    <t>ТК39</t>
+  </si>
+  <si>
+    <t>ТК40</t>
+  </si>
+  <si>
+    <t>Открыто приложение "Вхосписе", произведена авторизация и открыт экран "About", отключено интернет соединение.</t>
+  </si>
+  <si>
+    <t>1. Открылся экран "Main". Появилось всплывающее сообщение: "Something went wrong. Try again later".</t>
+  </si>
+  <si>
+    <t>Переход с экрана Main на экран News с помощью кнопки "All news". Негативный сценарий, потеря интернет соединения.</t>
+  </si>
+  <si>
+    <t>1. Нажать кнопку "All news".</t>
+  </si>
+  <si>
+    <t>1. Открылся экран "News". Появилось всплывающее сообщение: "Something went wrong. Try again later".</t>
+  </si>
+  <si>
+    <t>Открытие окна редактирования новостей. Негативный сценарий, потеря интернет соединения.</t>
+  </si>
+  <si>
+    <t>Открыто приложение "Вхосписе", произведена авторизация и отрыт экран "News", отключено интернет соединение.</t>
+  </si>
+  <si>
+    <t>1. Открылся экран "Control panel". Появилось всплывающее сообщение: "Something went wrong. Try again later".</t>
+  </si>
+  <si>
+    <t>Добавление новости. Негативный сценарий, потеря интернет соединения.</t>
+  </si>
+  <si>
+    <t>Открыто приложение "Вхосписе", произведена авторизация и отрыт экран "Control panel", отключено интернет соединение.</t>
+  </si>
+  <si>
+    <t>7. Появилось всплывающее сообщение: "Something went wrong. Try again later".</t>
+  </si>
+  <si>
+    <t>Редактирование новости. Негативный сценарий, потеря интернет соединения.</t>
+  </si>
+  <si>
+    <t>8. Появилось всплывающее сообщение: "Something went wrong. Try again later".</t>
+  </si>
+  <si>
     <t>Название тестового сценария</t>
-  </si>
-  <si>
-    <t>Описание если необходимо</t>
   </si>
   <si>
     <t>Предусловия если необходимы</t>
@@ -808,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -860,6 +1061,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1211,7 +1415,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="10" t="s">
@@ -1221,7 +1425,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>12</v>
@@ -1633,7 +1837,7 @@
       <c r="E33" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="14" t="s">
         <v>90</v>
       </c>
       <c r="G33" s="11" t="s">
@@ -1967,7 +2171,7 @@
       <c r="F56" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="G56" s="20" t="s">
+      <c r="G56" s="21" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2692,11 +2896,11 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="15"/>
-      <c r="B107" s="16"/>
-      <c r="C107" s="16"/>
-      <c r="D107" s="16"/>
-      <c r="E107" s="16"/>
+      <c r="A107" s="12"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
       <c r="F107" s="14" t="s">
         <v>213</v>
       </c>
@@ -2705,92 +2909,76 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="7" t="s">
+      <c r="A108" s="15"/>
+      <c r="B108" s="16"/>
+      <c r="C108" s="16"/>
+      <c r="D108" s="16"/>
+      <c r="E108" s="16"/>
+      <c r="F108" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G108" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B108" s="8" t="s">
+      <c r="B109" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C108" s="17"/>
-      <c r="D108" s="10" t="s">
+      <c r="C109" s="17"/>
+      <c r="D109" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E108" s="8" t="s">
+      <c r="E109" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="F108" s="14" t="s">
+      <c r="F109" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="G108" s="14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="15"/>
-      <c r="B109" s="16"/>
-      <c r="C109" s="16"/>
-      <c r="D109" s="16"/>
-      <c r="E109" s="16"/>
-      <c r="F109" s="14" t="s">
+      <c r="G109" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="G109" s="14" t="s">
-        <v>214</v>
-      </c>
     </row>
     <row r="110">
-      <c r="A110" s="7" t="s">
+      <c r="A110" s="12"/>
+      <c r="B110" s="13"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="B110" s="8" t="s">
+      <c r="G110" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="C110" s="17"/>
-      <c r="D110" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E110" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="F110" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="G110" s="14" t="s">
-        <v>212</v>
-      </c>
     </row>
     <row r="111">
-      <c r="A111" s="15"/>
-      <c r="B111" s="16"/>
-      <c r="C111" s="16"/>
-      <c r="D111" s="16"/>
-      <c r="E111" s="16"/>
+      <c r="A111" s="12"/>
+      <c r="B111" s="13"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
       <c r="F111" s="14" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G111" s="14" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="B112" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="C112" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="D112" s="17"/>
-      <c r="E112" s="17" t="s">
+      <c r="A112" s="12"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="F112" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="G112" s="19">
-        <v>1.0</v>
+      <c r="G112" s="11" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="113">
@@ -2799,37 +2987,45 @@
       <c r="C113" s="13"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
-      <c r="F113" s="19">
-        <v>2.0</v>
-      </c>
-      <c r="G113" s="19">
-        <v>2.0</v>
+      <c r="F113" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="G113" s="14" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="12"/>
-      <c r="B114" s="13"/>
-      <c r="C114" s="13"/>
-      <c r="D114" s="13"/>
-      <c r="E114" s="13"/>
-      <c r="F114" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="G114" s="19">
-        <v>3.0</v>
+      <c r="A114" s="15"/>
+      <c r="B114" s="16"/>
+      <c r="C114" s="16"/>
+      <c r="D114" s="16"/>
+      <c r="E114" s="16"/>
+      <c r="F114" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G114" s="14" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="12"/>
-      <c r="B115" s="13"/>
-      <c r="C115" s="13"/>
-      <c r="D115" s="13"/>
-      <c r="E115" s="13"/>
-      <c r="F115" s="19">
-        <v>4.0</v>
-      </c>
-      <c r="G115" s="19">
-        <v>4.0</v>
+      <c r="A115" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C115" s="17"/>
+      <c r="D115" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F115" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G115" s="14" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="116">
@@ -2838,11 +3034,11 @@
       <c r="C116" s="13"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
-      <c r="F116" s="19">
-        <v>5.0</v>
-      </c>
-      <c r="G116" s="19">
-        <v>5.0</v>
+      <c r="F116" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="G116" s="14" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="117">
@@ -2851,11 +3047,11 @@
       <c r="C117" s="13"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
-      <c r="F117" s="19">
-        <v>6.0</v>
-      </c>
-      <c r="G117" s="19">
-        <v>6.0</v>
+      <c r="F117" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="G117" s="14" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="118">
@@ -2864,11 +3060,11 @@
       <c r="C118" s="13"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
-      <c r="F118" s="19">
-        <v>7.0</v>
-      </c>
-      <c r="G118" s="19">
-        <v>7.0</v>
+      <c r="F118" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="G118" s="11" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="119">
@@ -2877,156 +3073,1187 @@
       <c r="C119" s="13"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
-      <c r="F119" s="19">
+      <c r="F119" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="G119" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="15"/>
+      <c r="B120" s="16"/>
+      <c r="C120" s="16"/>
+      <c r="D120" s="16"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G120" s="14" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C121" s="17"/>
+      <c r="D121" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E121" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="G121" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="15"/>
+      <c r="B122" s="16"/>
+      <c r="C122" s="16"/>
+      <c r="D122" s="16"/>
+      <c r="E122" s="16"/>
+      <c r="F122" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="G122" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C123" s="17"/>
+      <c r="D123" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E123" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F123" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G123" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="15"/>
+      <c r="B124" s="16"/>
+      <c r="C124" s="16"/>
+      <c r="D124" s="16"/>
+      <c r="E124" s="16"/>
+      <c r="F124" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="G124" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C125" s="17"/>
+      <c r="D125" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E125" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F125" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G125" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="12"/>
+      <c r="B126" s="13"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
+      <c r="F126" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="G126" s="14" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="15"/>
+      <c r="B127" s="16"/>
+      <c r="C127" s="16"/>
+      <c r="D127" s="16"/>
+      <c r="E127" s="16"/>
+      <c r="F127" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="G127" s="14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C128" s="17"/>
+      <c r="D128" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E128" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F128" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G128" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="12"/>
+      <c r="B129" s="13"/>
+      <c r="C129" s="13"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="13"/>
+      <c r="F129" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="G129" s="14" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="15"/>
+      <c r="B130" s="16"/>
+      <c r="C130" s="16"/>
+      <c r="D130" s="16"/>
+      <c r="E130" s="16"/>
+      <c r="F130" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="G130" s="14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C131" s="17"/>
+      <c r="D131" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E131" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F131" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G131" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="12"/>
+      <c r="B132" s="13"/>
+      <c r="C132" s="13"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="13"/>
+      <c r="F132" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G132" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="12"/>
+      <c r="B133" s="13"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="13"/>
+      <c r="F133" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G133" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="12"/>
+      <c r="B134" s="13"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="13"/>
+      <c r="F134" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="G134" s="14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="15"/>
+      <c r="B135" s="16"/>
+      <c r="C135" s="16"/>
+      <c r="D135" s="16"/>
+      <c r="E135" s="16"/>
+      <c r="F135" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="G135" s="14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C136" s="17"/>
+      <c r="D136" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E136" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F136" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G136" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="12"/>
+      <c r="B137" s="13"/>
+      <c r="C137" s="13"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="13"/>
+      <c r="F137" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G137" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="12"/>
+      <c r="B138" s="13"/>
+      <c r="C138" s="13"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
+      <c r="F138" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G138" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="12"/>
+      <c r="B139" s="13"/>
+      <c r="C139" s="13"/>
+      <c r="D139" s="13"/>
+      <c r="E139" s="13"/>
+      <c r="F139" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="G139" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="12"/>
+      <c r="B140" s="13"/>
+      <c r="C140" s="13"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
+      <c r="F140" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="G140" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="15"/>
+      <c r="B141" s="16"/>
+      <c r="C141" s="16"/>
+      <c r="D141" s="16"/>
+      <c r="E141" s="16"/>
+      <c r="F141" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="G141" s="14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C142" s="17"/>
+      <c r="D142" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E142" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F142" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G142" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="12"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
+      <c r="F143" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G143" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="12"/>
+      <c r="B144" s="13"/>
+      <c r="C144" s="13"/>
+      <c r="D144" s="13"/>
+      <c r="E144" s="13"/>
+      <c r="F144" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G144" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="12"/>
+      <c r="B145" s="13"/>
+      <c r="C145" s="13"/>
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
+      <c r="F145" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G145" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="12"/>
+      <c r="B146" s="13"/>
+      <c r="C146" s="13"/>
+      <c r="D146" s="13"/>
+      <c r="E146" s="13"/>
+      <c r="F146" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G146" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="12"/>
+      <c r="B147" s="13"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
+      <c r="F147" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G147" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="12"/>
+      <c r="B148" s="13"/>
+      <c r="C148" s="13"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="13"/>
+      <c r="F148" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="G148" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="15"/>
+      <c r="B149" s="16"/>
+      <c r="C149" s="16"/>
+      <c r="D149" s="16"/>
+      <c r="E149" s="16"/>
+      <c r="F149" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="G149" s="14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="150" ht="25.5" customHeight="1">
+      <c r="A150" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C150" s="17"/>
+      <c r="D150" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E150" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="F150" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G150" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="151" ht="44.25" customHeight="1">
+      <c r="A151" s="15"/>
+      <c r="B151" s="16"/>
+      <c r="C151" s="16"/>
+      <c r="D151" s="16"/>
+      <c r="E151" s="16"/>
+      <c r="F151" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G151" s="14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="152" ht="30.0" customHeight="1">
+      <c r="A152" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C152" s="17"/>
+      <c r="D152" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E152" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="F152" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G152" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="153" ht="41.25" customHeight="1">
+      <c r="A153" s="15"/>
+      <c r="B153" s="16"/>
+      <c r="C153" s="16"/>
+      <c r="D153" s="16"/>
+      <c r="E153" s="16"/>
+      <c r="F153" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G153" s="14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="154" ht="30.75" customHeight="1">
+      <c r="A154" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C154" s="17"/>
+      <c r="D154" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E154" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="F154" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G154" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="155" ht="48.0" customHeight="1">
+      <c r="A155" s="15"/>
+      <c r="B155" s="16"/>
+      <c r="C155" s="16"/>
+      <c r="D155" s="16"/>
+      <c r="E155" s="16"/>
+      <c r="F155" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G155" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="156" ht="31.5" customHeight="1">
+      <c r="A156" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B156" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C156" s="17"/>
+      <c r="D156" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E156" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="F156" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G156" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="157" ht="45.75" customHeight="1">
+      <c r="A157" s="15"/>
+      <c r="B157" s="16"/>
+      <c r="C157" s="16"/>
+      <c r="D157" s="16"/>
+      <c r="E157" s="16"/>
+      <c r="F157" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G157" s="14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="B158" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C158" s="19"/>
+      <c r="D158" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E158" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="F158" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G158" s="14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B159" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="C159" s="19"/>
+      <c r="D159" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E159" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="F159" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="G159" s="14" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B160" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="C160" s="19"/>
+      <c r="D160" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E160" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="F160" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G160" s="14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C161" s="17"/>
+      <c r="D161" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E161" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="F161" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G161" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="12"/>
+      <c r="B162" s="13"/>
+      <c r="C162" s="13"/>
+      <c r="D162" s="13"/>
+      <c r="E162" s="13"/>
+      <c r="F162" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G162" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="12"/>
+      <c r="B163" s="13"/>
+      <c r="C163" s="13"/>
+      <c r="D163" s="13"/>
+      <c r="E163" s="13"/>
+      <c r="F163" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G163" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="12"/>
+      <c r="B164" s="13"/>
+      <c r="C164" s="13"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="13"/>
+      <c r="F164" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G164" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="12"/>
+      <c r="B165" s="13"/>
+      <c r="C165" s="13"/>
+      <c r="D165" s="13"/>
+      <c r="E165" s="13"/>
+      <c r="F165" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="G165" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="12"/>
+      <c r="B166" s="13"/>
+      <c r="C166" s="13"/>
+      <c r="D166" s="13"/>
+      <c r="E166" s="13"/>
+      <c r="F166" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G166" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="15"/>
+      <c r="B167" s="16"/>
+      <c r="C167" s="16"/>
+      <c r="D167" s="16"/>
+      <c r="E167" s="16"/>
+      <c r="F167" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G167" s="14" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C168" s="17"/>
+      <c r="D168" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E168" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="F168" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G168" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="12"/>
+      <c r="B169" s="13"/>
+      <c r="C169" s="13"/>
+      <c r="D169" s="13"/>
+      <c r="E169" s="13"/>
+      <c r="F169" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G169" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="12"/>
+      <c r="B170" s="13"/>
+      <c r="C170" s="13"/>
+      <c r="D170" s="13"/>
+      <c r="E170" s="13"/>
+      <c r="F170" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G170" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="12"/>
+      <c r="B171" s="13"/>
+      <c r="C171" s="13"/>
+      <c r="D171" s="13"/>
+      <c r="E171" s="13"/>
+      <c r="F171" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="G171" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="12"/>
+      <c r="B172" s="13"/>
+      <c r="C172" s="13"/>
+      <c r="D172" s="13"/>
+      <c r="E172" s="13"/>
+      <c r="F172" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G172" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="12"/>
+      <c r="B173" s="13"/>
+      <c r="C173" s="13"/>
+      <c r="D173" s="13"/>
+      <c r="E173" s="13"/>
+      <c r="F173" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="G173" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="12"/>
+      <c r="B174" s="13"/>
+      <c r="C174" s="13"/>
+      <c r="D174" s="13"/>
+      <c r="E174" s="13"/>
+      <c r="F174" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G174" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="15"/>
+      <c r="B175" s="16"/>
+      <c r="C175" s="16"/>
+      <c r="D175" s="16"/>
+      <c r="E175" s="16"/>
+      <c r="F175" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G175" s="14" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B176" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C176" s="17"/>
+      <c r="D176" s="17"/>
+      <c r="E176" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="F176" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="G176" s="19">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="12"/>
+      <c r="B177" s="13"/>
+      <c r="C177" s="13"/>
+      <c r="D177" s="13"/>
+      <c r="E177" s="13"/>
+      <c r="F177" s="19">
+        <v>2.0</v>
+      </c>
+      <c r="G177" s="19">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="12"/>
+      <c r="B178" s="13"/>
+      <c r="C178" s="13"/>
+      <c r="D178" s="13"/>
+      <c r="E178" s="13"/>
+      <c r="F178" s="19">
+        <v>3.0</v>
+      </c>
+      <c r="G178" s="19">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="12"/>
+      <c r="B179" s="13"/>
+      <c r="C179" s="13"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="13"/>
+      <c r="F179" s="19">
+        <v>4.0</v>
+      </c>
+      <c r="G179" s="19">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="12"/>
+      <c r="B180" s="13"/>
+      <c r="C180" s="13"/>
+      <c r="D180" s="13"/>
+      <c r="E180" s="13"/>
+      <c r="F180" s="19">
+        <v>5.0</v>
+      </c>
+      <c r="G180" s="19">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="12"/>
+      <c r="B181" s="13"/>
+      <c r="C181" s="13"/>
+      <c r="D181" s="13"/>
+      <c r="E181" s="13"/>
+      <c r="F181" s="19">
+        <v>6.0</v>
+      </c>
+      <c r="G181" s="19">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="12"/>
+      <c r="B182" s="13"/>
+      <c r="C182" s="13"/>
+      <c r="D182" s="13"/>
+      <c r="E182" s="13"/>
+      <c r="F182" s="19">
+        <v>7.0</v>
+      </c>
+      <c r="G182" s="19">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="12"/>
+      <c r="B183" s="13"/>
+      <c r="C183" s="13"/>
+      <c r="D183" s="13"/>
+      <c r="E183" s="13"/>
+      <c r="F183" s="19">
         <v>8.0</v>
       </c>
-      <c r="G119" s="19">
+      <c r="G183" s="19">
         <v>8.0</v>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" s="12"/>
-      <c r="B120" s="13"/>
-      <c r="C120" s="13"/>
-      <c r="D120" s="13"/>
-      <c r="E120" s="13"/>
-      <c r="F120" s="19">
+    <row r="184">
+      <c r="A184" s="12"/>
+      <c r="B184" s="13"/>
+      <c r="C184" s="13"/>
+      <c r="D184" s="13"/>
+      <c r="E184" s="13"/>
+      <c r="F184" s="19">
         <v>9.0</v>
       </c>
-      <c r="G120" s="19">
+      <c r="G184" s="19">
         <v>9.0</v>
       </c>
     </row>
-    <row r="121">
-      <c r="A121" s="15"/>
-      <c r="B121" s="16"/>
-      <c r="C121" s="16"/>
-      <c r="D121" s="16"/>
-      <c r="E121" s="16"/>
-      <c r="F121" s="19">
+    <row r="185">
+      <c r="A185" s="15"/>
+      <c r="B185" s="16"/>
+      <c r="C185" s="16"/>
+      <c r="D185" s="16"/>
+      <c r="E185" s="16"/>
+      <c r="F185" s="19">
         <v>10.0</v>
       </c>
-      <c r="G121" s="19">
+      <c r="G185" s="19">
         <v>10.0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="115">
+  <mergeCells count="180">
+    <mergeCell ref="E150:E151"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="E128:E130"/>
+    <mergeCell ref="C128:C130"/>
+    <mergeCell ref="D128:D130"/>
+    <mergeCell ref="B128:B130"/>
+    <mergeCell ref="D125:D127"/>
+    <mergeCell ref="E125:E127"/>
+    <mergeCell ref="B125:B127"/>
+    <mergeCell ref="C125:C127"/>
+    <mergeCell ref="A128:A130"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="D136:D141"/>
+    <mergeCell ref="E136:E141"/>
+    <mergeCell ref="C136:C141"/>
+    <mergeCell ref="D131:D135"/>
+    <mergeCell ref="E131:E135"/>
+    <mergeCell ref="C131:C135"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="A142:A149"/>
+    <mergeCell ref="A136:A141"/>
+    <mergeCell ref="B136:B141"/>
+    <mergeCell ref="A131:A135"/>
+    <mergeCell ref="B131:B135"/>
+    <mergeCell ref="B142:B149"/>
+    <mergeCell ref="D150:D151"/>
+    <mergeCell ref="D142:D149"/>
+    <mergeCell ref="C142:C149"/>
+    <mergeCell ref="E142:E149"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="B27:B32"/>
     <mergeCell ref="C27:C32"/>
     <mergeCell ref="D27:D32"/>
     <mergeCell ref="E27:E32"/>
+    <mergeCell ref="C36:C45"/>
+    <mergeCell ref="D36:D45"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="D34:D35"/>
-    <mergeCell ref="B34:B35"/>
     <mergeCell ref="E34:E35"/>
-    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B36:B45"/>
+    <mergeCell ref="E36:E45"/>
+    <mergeCell ref="D53:D60"/>
+    <mergeCell ref="E53:E60"/>
+    <mergeCell ref="A36:A45"/>
+    <mergeCell ref="A46:A52"/>
     <mergeCell ref="B46:B52"/>
     <mergeCell ref="C46:C52"/>
-    <mergeCell ref="A36:A45"/>
-    <mergeCell ref="B36:B45"/>
-    <mergeCell ref="C36:C45"/>
-    <mergeCell ref="D36:D45"/>
-    <mergeCell ref="E36:E45"/>
-    <mergeCell ref="A46:A52"/>
     <mergeCell ref="D46:D52"/>
     <mergeCell ref="E46:E52"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
     <mergeCell ref="A53:A60"/>
-    <mergeCell ref="B53:B60"/>
-    <mergeCell ref="C53:C60"/>
-    <mergeCell ref="D53:D60"/>
-    <mergeCell ref="E53:E60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="E17:E18"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="B108:B109"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="E110:E111"/>
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="B110:B111"/>
-    <mergeCell ref="C112:C121"/>
-    <mergeCell ref="D112:D121"/>
-    <mergeCell ref="E112:E121"/>
-    <mergeCell ref="B112:B121"/>
-    <mergeCell ref="A112:A121"/>
-    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B53:B60"/>
+    <mergeCell ref="C53:C60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="A106:A108"/>
+    <mergeCell ref="B106:B108"/>
+    <mergeCell ref="C106:C108"/>
+    <mergeCell ref="D106:D108"/>
+    <mergeCell ref="E106:E108"/>
+    <mergeCell ref="B109:B114"/>
+    <mergeCell ref="E109:E114"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="B121:B122"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="A109:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="B115:B120"/>
+    <mergeCell ref="C115:C120"/>
+    <mergeCell ref="D115:D120"/>
+    <mergeCell ref="E115:E120"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="B123:B124"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="C109:C114"/>
+    <mergeCell ref="D109:D114"/>
+    <mergeCell ref="D152:D153"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="C152:C153"/>
+    <mergeCell ref="A152:A153"/>
+    <mergeCell ref="C154:C155"/>
+    <mergeCell ref="A154:A155"/>
+    <mergeCell ref="C67:C79"/>
+    <mergeCell ref="D67:D79"/>
+    <mergeCell ref="A65:A66"/>
     <mergeCell ref="B65:B66"/>
     <mergeCell ref="C65:C66"/>
-    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="D65:D66"/>
     <mergeCell ref="E65:E66"/>
+    <mergeCell ref="B67:B79"/>
     <mergeCell ref="E67:E79"/>
-    <mergeCell ref="D67:D79"/>
-    <mergeCell ref="C67:C79"/>
-    <mergeCell ref="B67:B79"/>
+    <mergeCell ref="B93:B105"/>
+    <mergeCell ref="C93:C105"/>
+    <mergeCell ref="D93:D105"/>
+    <mergeCell ref="E93:E105"/>
     <mergeCell ref="A67:A79"/>
+    <mergeCell ref="A80:A92"/>
+    <mergeCell ref="B80:B92"/>
+    <mergeCell ref="C80:C92"/>
+    <mergeCell ref="D80:D92"/>
     <mergeCell ref="E80:E92"/>
-    <mergeCell ref="D80:D92"/>
-    <mergeCell ref="C80:C92"/>
-    <mergeCell ref="B80:B92"/>
-    <mergeCell ref="A80:A92"/>
-    <mergeCell ref="B93:B105"/>
     <mergeCell ref="A93:A105"/>
-    <mergeCell ref="E93:E105"/>
-    <mergeCell ref="D93:D105"/>
-    <mergeCell ref="C93:C105"/>
-    <mergeCell ref="B106:B107"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="C110:C111"/>
-    <mergeCell ref="D110:D111"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="B156:B157"/>
+    <mergeCell ref="A156:A157"/>
+    <mergeCell ref="D154:D155"/>
+    <mergeCell ref="E154:E155"/>
+    <mergeCell ref="E156:E157"/>
+    <mergeCell ref="C156:C157"/>
+    <mergeCell ref="D156:D157"/>
+    <mergeCell ref="B176:B185"/>
+    <mergeCell ref="C176:C185"/>
+    <mergeCell ref="B161:B167"/>
+    <mergeCell ref="C161:C167"/>
+    <mergeCell ref="D161:D167"/>
+    <mergeCell ref="E161:E167"/>
+    <mergeCell ref="A176:A185"/>
+    <mergeCell ref="E176:E185"/>
+    <mergeCell ref="A161:A167"/>
+    <mergeCell ref="D168:D175"/>
+    <mergeCell ref="E168:E175"/>
+    <mergeCell ref="B168:B175"/>
+    <mergeCell ref="C168:C175"/>
+    <mergeCell ref="A168:A175"/>
+    <mergeCell ref="D176:D185"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>